<commit_message>
3NF, Updated table and data
</commit_message>
<xml_diff>
--- a/VectorDataInExcel-1NF.xlsx
+++ b/VectorDataInExcel-1NF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{F39FAA03-2BFE-49CF-9122-15144D823D4F}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{1AC70E95-5BA9-47A2-84C2-68E45A41E989}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7DCE2BE0-953A-4365-ADEC-B2ECAC53B523}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="189">
   <si>
     <t>Column1</t>
   </si>
@@ -604,10 +604,25 @@
     <t>Modem Status External</t>
   </si>
   <si>
-    <t>PK</t>
-  </si>
-  <si>
     <t xml:space="preserve">       PK</t>
+  </si>
+  <si>
+    <t>Partial Dependency</t>
+  </si>
+  <si>
+    <t>Transitive Dependency</t>
+  </si>
+  <si>
+    <t>(This would continue for all types)</t>
+  </si>
+  <si>
+    <t>From:</t>
+  </si>
+  <si>
+    <t>All these relate to a specific network and a specific antenna type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Transitive</t>
   </si>
 </sst>
 </file>
@@ -698,11 +713,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -829,6 +845,1842 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1495425</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Left Bracket 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBEAC78A-25C8-43B5-9206-7D4FC4CB9398}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="514350"/>
+          <a:ext cx="342900" cy="6648450"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Left Bracket 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2690D3D-6BB5-4B26-BD68-268EAB8C71DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="7172325"/>
+          <a:ext cx="323850" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Left Bracket 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D427F0EB-C89A-4F59-88F2-AED47510876E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="7343775"/>
+          <a:ext cx="323850" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Left Bracket 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E89BCCC-4996-426C-8FE2-4606FCDF1AF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="7515225"/>
+          <a:ext cx="323850" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Left Bracket 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A291937B-8EE1-4E43-B767-4A4FA632DB01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="7686675"/>
+          <a:ext cx="323850" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Left Bracket 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{224BB0BA-66AF-4DA0-9221-54D7106ADC9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="7896225"/>
+          <a:ext cx="323850" cy="2686050"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Right Bracket 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6043090-7E0E-48A6-8FE0-B6CEEF127329}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13182600" y="2390775"/>
+          <a:ext cx="428625" cy="4781550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Right Bracket 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52DCF420-2160-4C63-917B-7E9FCF2B8A41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13182600" y="3152775"/>
+          <a:ext cx="428625" cy="4019550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Right Bracket 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D69827B-9C83-470A-B699-4E39A5E2F01C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13182600" y="4133850"/>
+          <a:ext cx="428625" cy="3028950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Right Bracket 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBF8BFB4-AD02-4AA2-98EA-599A5270C3E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13173075" y="6219824"/>
+          <a:ext cx="428625" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A090F1E-5FE9-4A4E-9CCD-4EE28F3A3608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13687425" y="4886325"/>
+          <a:ext cx="428625" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C4BD12-192F-4440-8373-3A5385F0CAB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13182600" y="2390775"/>
+          <a:ext cx="266700" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E87ED526-9C10-4B0C-B43A-FA9CDA85AA0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13144500" y="3152775"/>
+          <a:ext cx="333375" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC61B60-C2F8-4298-A837-02E25A13FB52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13134975" y="4133850"/>
+          <a:ext cx="285750" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD38E30-AED5-4A33-BA38-EC3C765D1D6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13096875" y="6219825"/>
+          <a:ext cx="295275" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1495425</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E187BFE-3576-421F-9F93-EC92706F44C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="7134225"/>
+          <a:ext cx="228600" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1514475</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C41BA2-EDC7-4F40-B291-B1AF9979E92D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="7334250"/>
+          <a:ext cx="257175" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1514475</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E787390C-7171-40DF-BDA1-EBDBF00A8CB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247775" y="7505700"/>
+          <a:ext cx="266700" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4362AD-959B-4786-8F5D-DDBFCEA38C25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="7686675"/>
+          <a:ext cx="295275" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE8D5C76-A601-46A2-A87A-96F3ADC626D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1247775" y="7886700"/>
+          <a:ext cx="276225" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Arrow Connector 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF726075-D3DC-44A9-A79F-C4904416403D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1295400" y="10572750"/>
+          <a:ext cx="247650" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Left Bracket 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{294DB534-021C-4B73-BB62-DD7630FE155D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="523875"/>
+          <a:ext cx="104775" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1371601</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1466851</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Left Bracket 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1AED53-F000-45D9-B1C4-B5C530862E1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371601" y="285750"/>
+          <a:ext cx="95250" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1466851</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1495425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFCB428-FE7C-4CFB-BF9E-A19ED4167C02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466851" y="285750"/>
+          <a:ext cx="28574" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1381125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Arrow Connector 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C47C2E2D-6D48-4F31-8657-D9E02566DC74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1381125" y="838200"/>
+          <a:ext cx="152400" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1466851</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Arrow Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87C3A1DC-16F7-478B-9381-2E69B5768EB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466851" y="1009650"/>
+          <a:ext cx="76199" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Right Bracket 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13E7A72-8685-4CDD-8521-7A465123D5EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="7162800"/>
+          <a:ext cx="409575" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9F4D8E-EA09-452A-BF42-C341FE71B56A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13144500" y="8115300"/>
+          <a:ext cx="295275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Right Bracket 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9883B1F-F277-4455-A141-41BC350E494A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13220700" y="8115300"/>
+          <a:ext cx="390525" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF64D2F5-0C27-4243-930B-664192359394}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13163550" y="11553825"/>
+          <a:ext cx="257175" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Right Bracket 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{899B3868-7A18-4F6F-B3A2-DDE658F6F605}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13601701" y="10201274"/>
+          <a:ext cx="600074" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D019D29-BE1C-4352-BE28-EBC05A9C5637}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13154025" y="10553699"/>
+          <a:ext cx="447676" cy="9526"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Right Brace 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA0D3A3-6145-4739-96A7-CE4EB94C3744}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13268325" y="9039225"/>
+          <a:ext cx="304800" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1173,8 +3025,8 @@
   </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +3094,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1568,7 +3420,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>52</v>
       </c>
@@ -1591,7 +3443,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>55</v>
       </c>
@@ -1614,7 +3466,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>56</v>
       </c>
@@ -1637,7 +3489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>60</v>
       </c>
@@ -1660,7 +3512,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="B21" t="s">
         <v>61</v>
       </c>
@@ -1683,7 +3538,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>62</v>
       </c>
@@ -1706,7 +3561,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>65</v>
       </c>
@@ -1729,7 +3584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>66</v>
       </c>
@@ -1752,7 +3607,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>71</v>
       </c>
@@ -1775,7 +3630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>72</v>
       </c>
@@ -1797,8 +3652,11 @@
       <c r="H26" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K26" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>73</v>
       </c>
@@ -1820,8 +3678,11 @@
       <c r="H27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>75</v>
       </c>
@@ -1843,8 +3704,11 @@
       <c r="H28" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>76</v>
       </c>
@@ -1866,8 +3730,11 @@
       <c r="H29" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>78</v>
       </c>
@@ -1889,8 +3756,11 @@
       <c r="H30" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>80</v>
       </c>
@@ -1912,8 +3782,11 @@
       <c r="H31" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>82</v>
       </c>
@@ -1935,8 +3808,11 @@
       <c r="H32" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>84</v>
       </c>
@@ -1958,8 +3834,11 @@
       <c r="H33" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>87</v>
       </c>
@@ -1982,7 +3861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>88</v>
       </c>
@@ -2004,8 +3883,11 @@
       <c r="H35" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>89</v>
       </c>
@@ -2028,7 +3910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>90</v>
       </c>
@@ -2051,7 +3933,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>91</v>
       </c>
@@ -2074,7 +3956,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>94</v>
       </c>
@@ -2097,7 +3979,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>95</v>
       </c>
@@ -2120,7 +4002,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>97</v>
       </c>
@@ -2143,7 +4025,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>98</v>
       </c>
@@ -2166,7 +4048,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>99</v>
       </c>
@@ -2189,7 +4071,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>103</v>
       </c>
@@ -2212,7 +4094,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>104</v>
       </c>
@@ -2238,7 +4120,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>111</v>
       </c>
@@ -2261,7 +4143,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>112</v>
       </c>
@@ -2284,7 +4166,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>114</v>
       </c>
@@ -2307,7 +4189,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>121</v>
       </c>
@@ -2330,7 +4212,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>128</v>
       </c>
@@ -2353,7 +4235,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>134</v>
       </c>
@@ -2376,7 +4258,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>136</v>
       </c>
@@ -2399,7 +4281,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>140</v>
       </c>
@@ -2422,7 +4304,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>146</v>
       </c>
@@ -2444,8 +4326,11 @@
       <c r="H54" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K54" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>152</v>
       </c>
@@ -2468,7 +4353,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>154</v>
       </c>
@@ -2491,7 +4376,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>161</v>
       </c>
@@ -2514,7 +4399,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>163</v>
       </c>
@@ -2537,7 +4422,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>165</v>
       </c>
@@ -2560,7 +4445,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>170</v>
       </c>
@@ -2583,7 +4468,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>173</v>
       </c>
@@ -2606,7 +4491,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>177</v>
       </c>
@@ -2629,7 +4514,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>178</v>
       </c>
@@ -2652,7 +4537,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>180</v>
       </c>

</xml_diff>